<commit_message>
Recorded and edited taunt clips and an sfx. Tweaked script to accomodate.
</commit_message>
<xml_diff>
--- a/AssetSources/Voice Lines/VoiceLines.xlsx
+++ b/AssetSources/Voice Lines/VoiceLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\Voice Lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533EBFCB-C33A-44E0-80A3-798E671CD665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB13A407-7723-46FC-BA9B-5EAEDA39792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17835" windowHeight="20985" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="80">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -237,6 +237,45 @@
   </si>
   <si>
     <t>"Oh, look! My face is all exposed! Betchya cannae hit me!"</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Aggro</t>
+  </si>
+  <si>
+    <t>"You think you're tough!? I got some scrap for ya!"</t>
+  </si>
+  <si>
+    <t>KickYerArse</t>
+  </si>
+  <si>
+    <t>GotScrapForYa</t>
+  </si>
+  <si>
+    <t>"Now you see me!"</t>
+  </si>
+  <si>
+    <t>Seen</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>"Now you don't!"</t>
+  </si>
+  <si>
+    <t>NowYouDont</t>
+  </si>
+  <si>
+    <t>NowYouSee</t>
+  </si>
+  <si>
+    <t>"That's It! I'll kick yer arse!"</t>
   </si>
 </sst>
 </file>
@@ -281,7 +320,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -633,21 +693,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="119.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -658,10 +718,13 @@
         <v>59</v>
       </c>
       <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,10 +735,13 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -686,10 +752,13 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -700,10 +769,13 @@
         <v>60</v>
       </c>
       <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -714,10 +786,13 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -728,10 +803,13 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -742,10 +820,13 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -756,10 +837,13 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -770,10 +854,13 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -784,10 +871,13 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -798,10 +888,13 @@
         <v>60</v>
       </c>
       <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -812,10 +905,13 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -826,10 +922,13 @@
         <v>60</v>
       </c>
       <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -840,10 +939,13 @@
         <v>60</v>
       </c>
       <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -854,10 +956,13 @@
         <v>60</v>
       </c>
       <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -868,10 +973,13 @@
         <v>60</v>
       </c>
       <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -882,10 +990,13 @@
         <v>60</v>
       </c>
       <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -896,10 +1007,13 @@
         <v>60</v>
       </c>
       <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -910,10 +1024,13 @@
         <v>60</v>
       </c>
       <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -924,10 +1041,13 @@
         <v>60</v>
       </c>
       <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -938,10 +1058,13 @@
         <v>60</v>
       </c>
       <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -952,10 +1075,13 @@
         <v>60</v>
       </c>
       <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -966,10 +1092,13 @@
         <v>60</v>
       </c>
       <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -980,10 +1109,13 @@
         <v>60</v>
       </c>
       <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -994,10 +1126,13 @@
         <v>60</v>
       </c>
       <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1008,10 +1143,13 @@
         <v>60</v>
       </c>
       <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1022,10 +1160,13 @@
         <v>60</v>
       </c>
       <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1036,10 +1177,13 @@
         <v>60</v>
       </c>
       <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1050,10 +1194,13 @@
         <v>60</v>
       </c>
       <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
@@ -1064,10 +1211,13 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1078,16 +1228,87 @@
         <v>28</v>
       </c>
       <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" t="s">
         <v>62</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A31">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>(INDIRECT("B"&amp;ROW()) = "X")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B31">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>(INDIRECT("B"&amp;ROW())="X")</formula>
     </cfRule>

</xml_diff>

<commit_message>
More voice lines, more code, get ready for release.
</commit_message>
<xml_diff>
--- a/AssetSources/Voice Lines/VoiceLines.xlsx
+++ b/AssetSources/Voice Lines/VoiceLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\Voice Lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB13A407-7723-46FC-BA9B-5EAEDA39792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C63853-FB38-4C7D-BD0E-89DA3A053C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="135">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -122,9 +122,6 @@
     <t>AwfulBreath</t>
   </si>
   <si>
-    <t>Me</t>
-  </si>
-  <si>
     <t>PokeYerEye</t>
   </si>
   <si>
@@ -276,15 +273,191 @@
   </si>
   <si>
     <t>"That's It! I'll kick yer arse!"</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>"I hope this centipede eats your face!"</t>
+  </si>
+  <si>
+    <t>"Looks like you're being haunted! I hope you get possesed you useless pile of trash!"</t>
+  </si>
+  <si>
+    <t>YouDied</t>
+  </si>
+  <si>
+    <t>EmployeeDown</t>
+  </si>
+  <si>
+    <t>GhostGirl1</t>
+  </si>
+  <si>
+    <t>Thumper1</t>
+  </si>
+  <si>
+    <t>SpringHead1</t>
+  </si>
+  <si>
+    <t>Bracken1</t>
+  </si>
+  <si>
+    <t>Centipede1</t>
+  </si>
+  <si>
+    <t>"Hey look! Another employee. Go give him a hug!"</t>
+  </si>
+  <si>
+    <t>"Hey, you! I found some nuts for you to crack. They're over there!"</t>
+  </si>
+  <si>
+    <t>Spider1</t>
+  </si>
+  <si>
+    <t>Masked1</t>
+  </si>
+  <si>
+    <t>HoardingBug1</t>
+  </si>
+  <si>
+    <t>Jester1</t>
+  </si>
+  <si>
+    <t>Nutcracker1</t>
+  </si>
+  <si>
+    <t>"Hey! Employee! Ever been dissolved by a slime?"</t>
+  </si>
+  <si>
+    <t>"This Jester is hilarious! Go tell that joke to that employee over there! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"That's one scary butler! I'm glad I'm not you! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>Slime1</t>
+  </si>
+  <si>
+    <t>Butler1</t>
+  </si>
+  <si>
+    <t>"This one eats employees! I like it already!"</t>
+  </si>
+  <si>
+    <t>Maneater1</t>
+  </si>
+  <si>
+    <t>PlayerDeath</t>
+  </si>
+  <si>
+    <t>GargoyleDeath1</t>
+  </si>
+  <si>
+    <t>"These are my final words. I hate you. Hahahaha!"</t>
+  </si>
+  <si>
+    <t>PriorDeath</t>
+  </si>
+  <si>
+    <t>"a guy with a mask threw up on you and you fell over dead? maybe that possessed clone has more braincells than you!"</t>
+  </si>
+  <si>
+    <t>PriorMaskedDeath1</t>
+  </si>
+  <si>
+    <t>PriorManeaterDeath1</t>
+  </si>
+  <si>
+    <t>Sniker</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>"your parenting skills are worse than your survival skills - I didn't know that was even possible!"</t>
+  </si>
+  <si>
+    <t>"You're such a bad parent, even that maneater baby wants to kill you."</t>
+  </si>
+  <si>
+    <t>HoldManeater1</t>
+  </si>
+  <si>
+    <t>NearLedge1</t>
+  </si>
+  <si>
+    <t>NearLedge2</t>
+  </si>
+  <si>
+    <t>"Hey, clumsy! Betchya can't cross, you big baby!"</t>
+  </si>
+  <si>
+    <t>"Hey! Give the jump a try! What are you? Scared? Hahahaha!"</t>
+  </si>
+  <si>
+    <t>Deuce</t>
+  </si>
+  <si>
+    <t>"Hahahaha! You suck!"</t>
+  </si>
+  <si>
+    <t>YouSuck</t>
+  </si>
+  <si>
+    <t>"Another employee down! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"Hello, sir Bracken! He's over there! Hahahaha"</t>
+  </si>
+  <si>
+    <t>PriorFall1</t>
+  </si>
+  <si>
+    <t>"Remember that time you missed that jump and died? Great times."</t>
+  </si>
+  <si>
+    <t>ThePatienceToad</t>
+  </si>
+  <si>
+    <t>PajamaWearing</t>
+  </si>
+  <si>
+    <t>"What do you think of that, Mr. Pajama-Wearing, Basket-Face, Slipper-Wielding, Clipe-Dreep-Bauchle, Gether-Uping-Blate-Maw, Bleathering, Gomeril, Jessie, Oaf-Looking, Stauner, Nyaff, Plookie, Shan, Milk-Drinking, Soy-Faced Shilpit, Mim-Moothed, Sniveling, Worm-Eyed, Hotten-Blaugh, Vile-Stoochie, Callie-Breek-Tattie?"</t>
+  </si>
+  <si>
+    <t>"Hahahaha! You died!"</t>
+  </si>
+  <si>
+    <t>"Sit still and don't turn around. I want to watch that Spring Head maul you!"</t>
+  </si>
+  <si>
+    <t>"What a cute little Thumper! They're over there boy, go get em! Good boy!"</t>
+  </si>
+  <si>
+    <t>"The itsy bitsy spider ate the employees face. Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"Yippee! Hahahaha!"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -311,20 +484,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -336,32 +533,26 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,6 +565,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:E59" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:E59" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -693,34 +898,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="119.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="117.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -728,592 +935,983 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
         <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
+      <c r="B12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
+      <c r="B13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
+        <v>64</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
+      <c r="B17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" t="s">
-        <v>48</v>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" t="s">
-        <v>49</v>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>50</v>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>53</v>
+      <c r="B24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
+      <c r="B26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
+      <c r="B27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" t="s">
-        <v>38</v>
+      <c r="B28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" t="s">
-        <v>56</v>
+      <c r="B29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
+        <v>78</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" t="s">
         <v>69</v>
       </c>
-      <c r="E33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" t="s">
-        <v>78</v>
+        <v>129</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>77</v>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>(INDIRECT("B"&amp;ROW()) = "X")</formula>
+  <conditionalFormatting sqref="B60 A61:B1048576 A1:B59">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>(INDIRECT("B"&amp;ROW())="X")</formula>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>